<commit_message>
Added flowchart PNGs to assets folder
</commit_message>
<xml_diff>
--- a/backend/exports/approvals_report.xlsx
+++ b/backend/exports/approvals_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Approved For (User)</t>
   </si>
@@ -22,24 +22,45 @@
     <t>Approval Date</t>
   </si>
   <si>
+    <t>prajyotkankal9@gmail.com</t>
+  </si>
+  <si>
+    <t>1748856203722-414725785.png, 1749036756302-383338020.png, 1749036801330-106037180.png</t>
+  </si>
+  <si>
+    <t>6/17/2025</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
+    <t>1748799431337-109774176.jpg, 1748798941789-920707644.jpg</t>
+  </si>
+  <si>
+    <t>6/13/2025</t>
+  </si>
+  <si>
+    <t>6/12/2025</t>
+  </si>
+  <si>
+    <t>1749036756302-383338020.png</t>
+  </si>
+  <si>
+    <t>6/10/2025</t>
+  </si>
+  <si>
+    <t>1748798941789-920707644.jpg</t>
+  </si>
+  <si>
+    <t>1749030981363-555614522.png, 1749036756302-383338020.png</t>
+  </si>
+  <si>
     <t>1749036756302-383338020.png, 1749036801330-106037180.png</t>
   </si>
   <si>
-    <t>6/10/2025</t>
-  </si>
-  <si>
-    <t>prajyotkankal9@gmail.com</t>
-  </si>
-  <si>
     <t>1749030981363-555614522.png, 1749036740156-172730154.png</t>
   </si>
   <si>
-    <t>1748798941789-920707644.jpg</t>
-  </si>
-  <si>
     <t>6/9/2025</t>
   </si>
   <si>
@@ -74,9 +95,6 @@
   </si>
   <si>
     <t>6/2/2025</t>
-  </si>
-  <si>
-    <t>1748799431337-109774176.jpg, 1748798941789-920707644.jpg</t>
   </si>
   <si>
     <t>1748856203722-414725785.png</t>
@@ -456,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -489,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -508,10 +526,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,21 +537,21 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,21 +559,21 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,7 +581,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -571,57 +589,123 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made UI changes and additional functionalities
</commit_message>
<xml_diff>
--- a/backend/exports/approvals_report.xlsx
+++ b/backend/exports/approvals_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>Approved For (User)</t>
   </si>
@@ -25,97 +25,76 @@
     <t>prajyotkankal12@gmail.com</t>
   </si>
   <si>
+    <t>1748856203722-414725785.png, 1749030981363-555614522.png, 1749036723774-181764139.png</t>
+  </si>
+  <si>
+    <t>7/2/2025</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>1751355478348-902190519.jpg, 1751355478366-389058481.jpg, 1751355478330-519983988.jpg</t>
+  </si>
+  <si>
+    <t>prajyotkankal9@gmail.com</t>
+  </si>
+  <si>
+    <t>1749030981363-555614522.png, 1748856203722-414725785.png, 1749036723774-181764139.png</t>
+  </si>
+  <si>
+    <t>1748799431337-109774176.jpg, 1748798941789-920707644.jpg</t>
+  </si>
+  <si>
+    <t>1748856203722-414725785.png</t>
+  </si>
+  <si>
+    <t>Invalid Date</t>
+  </si>
+  <si>
+    <t>1748798941789-920707644.jpg, 1748799431337-109774176.jpg</t>
+  </si>
+  <si>
+    <t>1748798941789-920707644.jpg</t>
+  </si>
+  <si>
+    <t>1749036723774-181764139.png, 1749036740156-172730154.png, 1749036756302-383338020.png</t>
+  </si>
+  <si>
+    <t>1748856203722-414725785.png, 1749030981363-555614522.png</t>
+  </si>
+  <si>
+    <t>1749030981363-555614522.png, 1749036740156-172730154.png, 1749036756302-383338020.png</t>
+  </si>
+  <si>
+    <t>sanketnk1401@gmail.com</t>
+  </si>
+  <si>
+    <t>1749030981363-555614522.png, 1749036740156-172730154.png</t>
+  </si>
+  <si>
+    <t>1749036756302-383338020.png, 1749036801330-106037180.png</t>
+  </si>
+  <si>
+    <t>1749030981363-555614522.png, 1749036756302-383338020.png</t>
+  </si>
+  <si>
+    <t>1749036756302-383338020.png</t>
+  </si>
+  <si>
+    <t>1748856203722-414725785.png, 1749036756302-383338020.png, 1749036801330-106037180.png</t>
+  </si>
+  <si>
+    <t>1749036860469-671098807.png, 1749036801330-106037180.png, 1749036756302-383338020.png, 1749036723774-181764139.png, 1749030981363-555614522.png, 1749036740156-172730154.png</t>
+  </si>
+  <si>
+    <t>1749036723774-181764139.png, 1749036740156-172730154.png, 1749495188737-684413652.png</t>
+  </si>
+  <si>
     <t>1749036723774-181764139.png, 1749030981363-555614522.png, 1748856203722-414725785.png</t>
   </si>
   <si>
-    <t>7/1/2025</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>1749036723774-181764139.png, 1749036740156-172730154.png, 1749495188737-684413652.png</t>
-  </si>
-  <si>
-    <t>6/24/2025</t>
-  </si>
-  <si>
-    <t>prajyotkankal9@gmail.com</t>
-  </si>
-  <si>
-    <t>1749036860469-671098807.png, 1749036801330-106037180.png, 1749036756302-383338020.png, 1749036723774-181764139.png, 1749030981363-555614522.png, 1749036740156-172730154.png</t>
-  </si>
-  <si>
-    <t>6/20/2025</t>
-  </si>
-  <si>
-    <t>1748856203722-414725785.png, 1749036756302-383338020.png, 1749036801330-106037180.png</t>
-  </si>
-  <si>
-    <t>6/17/2025</t>
-  </si>
-  <si>
-    <t>1748799431337-109774176.jpg, 1748798941789-920707644.jpg</t>
-  </si>
-  <si>
-    <t>6/13/2025</t>
-  </si>
-  <si>
-    <t>6/12/2025</t>
-  </si>
-  <si>
-    <t>1749036756302-383338020.png</t>
-  </si>
-  <si>
-    <t>6/10/2025</t>
-  </si>
-  <si>
-    <t>1748798941789-920707644.jpg</t>
-  </si>
-  <si>
-    <t>1749030981363-555614522.png, 1749036756302-383338020.png</t>
-  </si>
-  <si>
-    <t>1749036756302-383338020.png, 1749036801330-106037180.png</t>
-  </si>
-  <si>
-    <t>1749030981363-555614522.png, 1749036740156-172730154.png</t>
-  </si>
-  <si>
-    <t>6/9/2025</t>
-  </si>
-  <si>
-    <t>sanketnk1401@gmail.com</t>
-  </si>
-  <si>
-    <t>1749036723774-181764139.png, 1749036740156-172730154.png, 1749036756302-383338020.png</t>
-  </si>
-  <si>
-    <t>6/7/2025</t>
-  </si>
-  <si>
-    <t>1749030981363-555614522.png, 1749036740156-172730154.png, 1749036756302-383338020.png</t>
-  </si>
-  <si>
-    <t>6/6/2025</t>
-  </si>
-  <si>
-    <t>1748856203722-414725785.png, 1749030981363-555614522.png</t>
-  </si>
-  <si>
-    <t>6/5/2025</t>
-  </si>
-  <si>
-    <t>1748798941789-920707644.jpg, 1748799431337-109774176.jpg</t>
-  </si>
-  <si>
-    <t>6/4/2025</t>
-  </si>
-  <si>
-    <t>6/2/2025</t>
-  </si>
-  <si>
-    <t>1748856203722-414725785.png</t>
+    <t>1751355478330-519983988.jpg, 1751355478348-902190519.jpg, 1751355478353-571790688.jpg</t>
   </si>
 </sst>
 </file>
@@ -492,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C29"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,238 +504,293 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>